<commit_message>
Switched Bill of Materials to newer version
Signed-off-by: Grant Haataja <grant.haataja@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Avionics/BillOfMaterials.xlsx
+++ b/docs/Avionics/BillOfMaterials.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARC\Research\Budgeting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B94215-1910-4008-8C76-BD99BF6A758C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10290" xr2:uid="{AF1B4D74-F097-48E8-B78F-81A8203A77D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -59,19 +58,31 @@
     <t>https://www.sancloud.co.uk/?page_id=1028&amp;model_number=BBE-WiFi-V1G</t>
   </si>
   <si>
-    <t>Test flight computer (clrnc)</t>
-  </si>
-  <si>
-    <t>https://www.sancloud.co.uk/?page_id=1028&amp;model_number=BBE-WiFi-V1G-Clearance</t>
-  </si>
-  <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micro Controller </t>
+  </si>
+  <si>
+    <t>Adafruit BNO055</t>
+  </si>
+  <si>
+    <t>Accelerometer</t>
+  </si>
+  <si>
+    <t>SparkFun MS5803-14BA</t>
+  </si>
+  <si>
+    <t>Barometer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -121,9 +132,12 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,15 +153,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6EA9CA4F-46ED-438F-9969-22DB344141D0}" name="Table1" displayName="Table1" ref="B2:G5" totalsRowCount="1">
-  <autoFilter ref="B2:G4" xr:uid="{E8EC465C-2308-449D-A04A-228BAAB2F7BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:G10" totalsRowCount="1">
+  <autoFilter ref="B2:G9"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{FA960FED-9B77-462D-8B7B-5F21B4E47FD1}" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{6C68167F-2D91-4F8C-B7AA-653DA993ADC8}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{CED91CBD-EB77-4032-85AF-586A9E48D94B}" name="Price per" totalsRowFunction="average" totalsRowDxfId="0" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{9A1C8CFF-D5BA-408E-A061-0F1B72679E24}" name="Link to purchase"/>
-    <tableColumn id="5" xr3:uid="{413D1EC0-0713-42ED-949D-C368B8DBD795}" name="Quantity" totalsRowFunction="sum"/>
-    <tableColumn id="6" xr3:uid="{4AA96682-8667-4A55-B5AE-F507E12D3315}" name="Price total" totalsRowFunction="sum" dataCellStyle="Currency" totalsRowCellStyle="Currency">
+    <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="Price per" totalsRowFunction="average" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="4" name="Link to purchase"/>
+    <tableColumn id="5" name="Quantity" totalsRowFunction="sum"/>
+    <tableColumn id="6" name="Price total" totalsRowFunction="sum" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>D3*F3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -451,24 +465,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376E5456-2493-4BC8-9522-4010F7C56592}">
-  <dimension ref="B2:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -488,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -509,42 +523,93 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
+        <v>6.59</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G4" s="1">
         <f>D4*F4</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+        <v>52.72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <f>D5*F5</f>
+        <v>174.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
+        <v>59.95</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <f>D6*F6</f>
+        <v>299.75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <f>D7*F7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <f>D8*F8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <f>D9*F9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
         <f>SUBTOTAL(101,Table1[Price per])</f>
-        <v>73</v>
-      </c>
-      <c r="F5">
+        <v>44.372500000000002</v>
+      </c>
+      <c r="F10">
         <f>SUBTOTAL(109,Table1[Quantity])</f>
-        <v>22</v>
-      </c>
-      <c r="G5" s="2">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2">
         <f>SUBTOTAL(109,Table1[Price total])</f>
-        <v>1666</v>
+        <v>2123.2200000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>